<commit_message>
added data and modified readme
</commit_message>
<xml_diff>
--- a/data/workout_sleep_patterns.xlsx
+++ b/data/workout_sleep_patterns.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ralhp\Documents\Sync\Sleep-and-Workout\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rkellazar/Documents/Sync/Sleep-and-Workout/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{75336420-89B8-4F25-BD96-2FEB687F7A00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8313FF1-07E8-264A-B516-22A7BAC5B034}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{67FC1435-AE0F-40B2-99BD-F9A897E8DB65}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{67FC1435-AE0F-40B2-99BD-F9A897E8DB65}"/>
   </bookViews>
   <sheets>
     <sheet name="workout_sleep" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>date</t>
   </si>
@@ -50,9 +50,6 @@
     <t>light_sleep</t>
   </si>
   <si>
-    <t>rem_sleep</t>
-  </si>
-  <si>
     <t>deep_sleep</t>
   </si>
   <si>
@@ -60,6 +57,18 @@
   </si>
   <si>
     <t>sleep_duration</t>
+  </si>
+  <si>
+    <t>score</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>full body</t>
+  </si>
+  <si>
+    <t>awakenings</t>
   </si>
 </sst>
 </file>
@@ -411,26 +420,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EAD3661-C221-4C74-B2C6-89D3CAAB4E71}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView tabSelected="1" zoomScale="179" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.42578125" customWidth="1"/>
+    <col min="1" max="1" width="10.1640625" customWidth="1"/>
+    <col min="2" max="2" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -438,22 +447,36 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
       </c>
       <c r="H1" t="s">
         <v>3</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>119</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>